<commit_message>
Lab6 lucru la scenarii testare
</commit_message>
<xml_diff>
--- a/Metings_General/Raport_lab6.xlsx
+++ b/Metings_General/Raport_lab6.xlsx
@@ -55,12 +55,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -112,16 +120,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent2" xfId="1" builtinId="34"/>
@@ -406,7 +415,7 @@
   <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +473,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -571,7 +580,9 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2">
+        <v>31</v>
+      </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>

</xml_diff>